<commit_message>
Export excel config file
</commit_message>
<xml_diff>
--- a/Assets/NoUploadAssets/Configs/ExcelFiles/Character.xlsx
+++ b/Assets/NoUploadAssets/Configs/ExcelFiles/Character.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="127">
   <si>
     <t>//Use "#------&gt;" to start and "#&lt;------" to stop payload.</t>
   </si>
@@ -300,10 +300,145 @@
     <t>m01</t>
   </si>
   <si>
+    <t>Green Goblin</t>
+  </si>
+  <si>
+    <t>Assets/HotupdateAssets/Prefabs/Monster/goblin_01.prefab</t>
+  </si>
+  <si>
     <t>m02</t>
   </si>
   <si>
+    <t>Red Machine Goblin</t>
+  </si>
+  <si>
+    <t>Assets/HotupdateAssets/Prefabs/Monster/goblin_02.prefab</t>
+  </si>
+  <si>
     <t>m03</t>
+  </si>
+  <si>
+    <t>Blue Goblin</t>
+  </si>
+  <si>
+    <t>Assets/HotupdateAssets/Prefabs/Monster/goblin_03.prefab</t>
+  </si>
+  <si>
+    <t>m04</t>
+  </si>
+  <si>
+    <t>Orange Machine Goblin</t>
+  </si>
+  <si>
+    <t>Assets/HotupdateAssets/Prefabs/Monster/goblin_04.prefab</t>
+  </si>
+  <si>
+    <t>m05</t>
+  </si>
+  <si>
+    <t>Normal Hobgoblin</t>
+  </si>
+  <si>
+    <t>Assets/HotupdateAssets/Prefabs/Monster/hobgoblin_01.prefab</t>
+  </si>
+  <si>
+    <t>m06</t>
+  </si>
+  <si>
+    <t>Blue Hobgoblin</t>
+  </si>
+  <si>
+    <t>Assets/HotupdateAssets/Prefabs/Monster/hobgoblin_02.prefab</t>
+  </si>
+  <si>
+    <t>m07</t>
+  </si>
+  <si>
+    <t>Red Hobgoblin</t>
+  </si>
+  <si>
+    <t>Assets/HotupdateAssets/Prefabs/Monster/hobgoblin_03.prefab</t>
+  </si>
+  <si>
+    <t>m08</t>
+  </si>
+  <si>
+    <t>Green Hobgoblin</t>
+  </si>
+  <si>
+    <t>Assets/HotupdateAssets/Prefabs/Monster/hobgoblin_04.prefab</t>
+  </si>
+  <si>
+    <t>m09</t>
+  </si>
+  <si>
+    <t>Normal Troll</t>
+  </si>
+  <si>
+    <t>Assets/HotupdateAssets/Prefabs/Monster/troll_01.prefab</t>
+  </si>
+  <si>
+    <t>m10</t>
+  </si>
+  <si>
+    <t>Red Troll</t>
+  </si>
+  <si>
+    <t>Assets/HotupdateAssets/Prefabs/Monster/troll_02.prefab</t>
+  </si>
+  <si>
+    <t>m11</t>
+  </si>
+  <si>
+    <t>Blue Troll</t>
+  </si>
+  <si>
+    <t>Assets/HotupdateAssets/Prefabs/Monster/troll_03.prefab</t>
+  </si>
+  <si>
+    <t>m12</t>
+  </si>
+  <si>
+    <t>Green Troll</t>
+  </si>
+  <si>
+    <t>Assets/HotupdateAssets/Prefabs/Monster/troll_04.prefab</t>
+  </si>
+  <si>
+    <t>m13</t>
+  </si>
+  <si>
+    <t>Normal Wolf</t>
+  </si>
+  <si>
+    <t>Assets/HotupdateAssets/Prefabs/Monster/wolf_01.prefab</t>
+  </si>
+  <si>
+    <t>m14</t>
+  </si>
+  <si>
+    <t>Blue Wolf</t>
+  </si>
+  <si>
+    <t>Assets/HotupdateAssets/Prefabs/Monster/wolf_02.prefab</t>
+  </si>
+  <si>
+    <t>m15</t>
+  </si>
+  <si>
+    <t>Orange Wolf</t>
+  </si>
+  <si>
+    <t>Assets/HotupdateAssets/Prefabs/Monster/wolf_03.prefab</t>
+  </si>
+  <si>
+    <t>m16</t>
+  </si>
+  <si>
+    <t>Dark Wolf</t>
+  </si>
+  <si>
+    <t>Assets/HotupdateAssets/Prefabs/Monster/wolf_04.prefab</t>
   </si>
 </sst>
 </file>
@@ -316,7 +451,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,13 +461,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -809,152 +937,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -964,7 +1092,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1299,7 +1426,7 @@
   <cols>
     <col min="1" max="1" width="13.247619047619" customWidth="1"/>
     <col min="2" max="2" width="6" customWidth="1"/>
-    <col min="3" max="3" width="18.4285714285714" style="9" customWidth="1"/>
+    <col min="3" max="3" width="18.4285714285714" style="5" customWidth="1"/>
     <col min="4" max="4" width="15.7142857142857" customWidth="1"/>
     <col min="5" max="5" width="11.3714285714286" customWidth="1"/>
     <col min="6" max="6" width="10.5047619047619" customWidth="1"/>
@@ -1547,7 +1674,7 @@
       <c r="D7" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="9">
         <v>133133133</v>
       </c>
       <c r="F7" s="5">
@@ -1623,7 +1750,7 @@
       <c r="J8" s="5">
         <v>569.891</v>
       </c>
-      <c r="K8" s="12" t="s">
+      <c r="K8" s="11" t="s">
         <v>55</v>
       </c>
       <c r="L8" s="5" t="s">
@@ -1691,7 +1818,7 @@
       <c r="N9" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="O9" s="12" t="s">
+      <c r="O9" s="11" t="s">
         <v>65</v>
       </c>
       <c r="P9" s="5">
@@ -1711,7 +1838,6 @@
         <v>66</v>
       </c>
       <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -1725,7 +1851,7 @@
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
-      <c r="O10" s="12"/>
+      <c r="O10" s="11"/>
       <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
@@ -1764,7 +1890,7 @@
       <c r="J11" s="5">
         <v>571.891</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="K11" s="11" t="s">
         <v>68</v>
       </c>
       <c r="L11" s="5" t="s">
@@ -1820,7 +1946,7 @@
       <c r="J12" s="5">
         <v>572.891</v>
       </c>
-      <c r="K12" s="12" t="s">
+      <c r="K12" s="11" t="s">
         <v>73</v>
       </c>
       <c r="L12" s="5" t="s">
@@ -1851,12 +1977,11 @@
       <c r="A13" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C13" s="11"/>
+      <c r="C13" s="10"/>
     </row>
     <row r="14" spans="1:22">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -1880,7 +2005,6 @@
     <row r="15" spans="1:22">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
@@ -1904,7 +2028,6 @@
     <row r="16" spans="1:22">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -1928,7 +2051,6 @@
     <row r="17" spans="1:22">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -1952,7 +2074,6 @@
     <row r="18" spans="1:22">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -1976,7 +2097,6 @@
     <row r="19" spans="1:22">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -2000,7 +2120,6 @@
     <row r="20" spans="1:22">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -2024,7 +2143,6 @@
     <row r="21" spans="1:22">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -2055,13 +2173,16 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A3:C11"/>
+  <dimension ref="A3:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
+  <cols>
+    <col min="2" max="2" width="23.8571428571429" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
@@ -2096,35 +2217,180 @@
       <c r="A6" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="C6" s="5" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>46</v>
+        <v>83</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="5" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="6" t="s">
         <v>78</v>
       </c>
     </row>

</xml_diff>